<commit_message>
mudanças na modelagem dos dados
</commit_message>
<xml_diff>
--- a/Gestor de estoque/Banco de dados.xlsx
+++ b/Gestor de estoque/Banco de dados.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleyb\WorkSpace\BroCode\Gestor de estoque\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\BroCODE\Gestor de estoque\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>usuario</t>
   </si>
@@ -80,9 +80,6 @@
     <t>id produto</t>
   </si>
   <si>
-    <t>id cliente</t>
-  </si>
-  <si>
     <t>preço venda</t>
   </si>
   <si>
@@ -120,12 +117,21 @@
   </si>
   <si>
     <t>id loja</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>id usuario</t>
+  </si>
+  <si>
+    <t>tipo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,23 +477,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="16.375" customWidth="1"/>
+    <col min="7" max="7" width="16.875" customWidth="1"/>
+    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -536,7 +543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -547,7 +554,7 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -559,13 +566,10 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -573,36 +577,36 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -611,10 +615,28 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tabelas:cliente venda loja produto registro
</commit_message>
<xml_diff>
--- a/Gestor de estoque/Banco de dados.xlsx
+++ b/Gestor de estoque/Banco de dados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>usuario</t>
   </si>
@@ -119,13 +119,19 @@
     <t>id loja</t>
   </si>
   <si>
-    <t>log</t>
-  </si>
-  <si>
     <t>id usuario</t>
   </si>
   <si>
     <t>tipo</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>registro</t>
+  </si>
+  <si>
+    <t>id venda</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,19 +626,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>